<commit_message>
Added List Named Items, Get Named Item and Named Item Range
</commit_message>
<xml_diff>
--- a/src/ExcelRESTExplorer.UWP/Content/Template.xlsx
+++ b/src/ExcelRESTExplorer.UWP/Content/Template.xlsx
@@ -1,19 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="BooleanConstant">FALSE</definedName>
+    <definedName name="Categories">Sheet3!$A$1:$A$4</definedName>
+    <definedName name="ChartData">Sheet3!$A$1:$B$4</definedName>
+    <definedName name="Counts">Sheet3!$B$1:$B$4</definedName>
+    <definedName name="DoubleConstant">5.5</definedName>
+    <definedName name="Formula">SUM(Sheet3!$B$2:$B$4)</definedName>
+    <definedName name="Hidden">Sheet4!$A$1</definedName>
+    <definedName name="IntegerConstant">100</definedName>
+    <definedName name="StringConstant">"Hello World"</definedName>
+  </definedNames>
   <calcPr calcId="171026"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -102,6 +114,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>This cell is hidden</t>
   </si>
 </sst>
 </file>
@@ -4084,7 +4099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4833,7 +4848,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4874,4 +4889,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>